<commit_message>
Controle - Sprint 7
</commit_message>
<xml_diff>
--- a/Administracao/Controle/presencas_e_entregas.xlsx
+++ b/Administracao/Controle/presencas_e_entregas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="36">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -1188,14 +1188,18 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="3.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="2.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,8 +1259,12 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1283,8 +1291,12 @@
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1311,8 +1323,12 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1339,8 +1355,12 @@
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1367,8 +1387,12 @@
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1395,8 +1419,12 @@
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1423,8 +1451,12 @@
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1451,8 +1483,12 @@
       <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1479,8 +1515,12 @@
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1507,8 +1547,12 @@
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1535,8 +1579,12 @@
       <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1563,8 +1611,12 @@
       <c r="F13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1591,8 +1643,12 @@
       <c r="F14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1619,8 +1675,12 @@
       <c r="F15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1647,8 +1707,12 @@
       <c r="F16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1675,8 +1739,12 @@
       <c r="F17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1703,8 +1771,12 @@
       <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1731,8 +1803,12 @@
       <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1759,8 +1835,12 @@
       <c r="F20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1787,8 +1867,12 @@
       <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1815,8 +1899,12 @@
       <c r="F22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>

</xml_diff>